<commit_message>
main plot function improvements and code comments
</commit_message>
<xml_diff>
--- a/inst/extdata/variable_defaults_and_help.xlsx
+++ b/inst/extdata/variable_defaults_and_help.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25003"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au530301_uni_au_dk/Documents/Vedhæftede filer/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{29142EC1-9537-924B-9CDE-F483343A11FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1132E0B0-956E-FC47-B69C-E91FBEE8D2C9}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{29142EC1-9537-924B-9CDE-F483343A11FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00672137-C049-5845-9EC4-4A364C4636F6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{E0DFC8D9-2769-CD42-9190-B3351BDE6F8D}"/>
   </bookViews>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -649,6 +651,12 @@
     <t>panel_separator</t>
   </si>
   <si>
+    <t>Vertical and Horizontal Line-Separators</t>
+  </si>
+  <si>
+    <t>Specify if vertical, horizontal line-separators should be displayed in order to clearly separate panels. Activated by default for vertical but not horizontal. Horizontal line-separators will only be displayed if 'Dataset Spacers' is ticked.</t>
+  </si>
+  <si>
     <t>separators_colors</t>
   </si>
   <si>
@@ -1052,19 +1060,13 @@
   </si>
   <si>
     <t>Shading opacity. Provide numeric value between 0 and 1. However, using a value  &lt;0.2 is recommended.</t>
-  </si>
-  <si>
-    <t>Horizontal and Vertical Line-Separators</t>
-  </si>
-  <si>
-    <t>Specify if horizontal,vertical line-separators should be displayed in order to clearly separate panels. Activated by default for vertical but not horizontal. Horizontal line-separators will only be displayed if 'Dataset Spacers' is ticked.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1472,24 +1474,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="98" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="5" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="27.875" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="4" max="5" width="22.375" customWidth="1"/>
     <col min="6" max="6" width="30.5" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="67.5" customWidth="1"/>
-    <col min="9" max="9" width="255.6640625" customWidth="1"/>
-    <col min="10" max="35" width="10.83203125"/>
+    <col min="9" max="9" width="255.625" customWidth="1"/>
+    <col min="10" max="35" width="10.875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1518,7 +1520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1547,7 +1549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1601,7 +1603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1628,7 +1630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1655,7 +1657,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1682,7 +1684,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1736,7 +1738,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1763,7 +1765,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1790,7 +1792,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1817,7 +1819,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1871,7 +1873,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1898,7 +1900,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1978,7 +1980,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -2005,7 +2007,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -2031,7 +2033,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -2058,7 +2060,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -2085,7 +2087,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -2139,7 +2141,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -2166,7 +2168,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -2193,7 +2195,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -2220,7 +2222,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2249,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>130</v>
       </c>
@@ -2274,7 +2276,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>130</v>
       </c>
@@ -2301,7 +2303,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
@@ -2330,7 +2332,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>130</v>
       </c>
@@ -2357,7 +2359,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>130</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>130</v>
       </c>
@@ -2411,7 +2413,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>130</v>
       </c>
@@ -2438,7 +2440,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>130</v>
       </c>
@@ -2465,7 +2467,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -2492,7 +2494,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -2519,7 +2521,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -2546,7 +2548,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
@@ -2573,7 +2575,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
@@ -2600,7 +2602,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
@@ -2627,7 +2629,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
@@ -2708,7 +2710,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
@@ -2735,7 +2737,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -2756,72 +2758,72 @@
         <v>203</v>
       </c>
       <c r="H47" t="s">
-        <v>339</v>
+        <v>204</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="8" t="s">
         <v>162</v>
       </c>
       <c r="G48" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H48" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="8" t="s">
         <v>162</v>
       </c>
       <c r="G49" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H49" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>18</v>
@@ -2834,75 +2836,75 @@
         <v>162</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="8" t="s">
         <v>162</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="8" t="s">
         <v>162</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>34</v>
@@ -2912,24 +2914,24 @@
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>34</v>
@@ -2939,24 +2941,24 @@
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>24</v>
@@ -2966,24 +2968,24 @@
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>34</v>
@@ -2993,78 +2995,78 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G56" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H56" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E57" s="6"/>
       <c r="F57" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G57" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="H57" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G58" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="H58" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>34</v>
@@ -3074,24 +3076,24 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G59" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="H59" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C60" t="s">
         <v>34</v>
@@ -3101,78 +3103,78 @@
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="9" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G60" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="H60" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C61" t="s">
         <v>34</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="9" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G61" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H61" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="9" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G62" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="H62" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C63" t="s">
         <v>34</v>
@@ -3182,53 +3184,53 @@
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="9" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G63" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H63" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D64" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="I64" s="10" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="B65" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>18</v>
@@ -3238,24 +3240,24 @@
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>18</v>
@@ -3265,24 +3267,24 @@
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>18</v>
@@ -3292,24 +3294,24 @@
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>18</v>
@@ -3319,24 +3321,24 @@
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>18</v>
@@ -3346,78 +3348,78 @@
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="I70" s="10" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G71" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H71" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>34</v>
@@ -3427,51 +3429,51 @@
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G72" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H72" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E73" s="6"/>
       <c r="F73" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G73" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H73" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>34</v>
@@ -3481,24 +3483,24 @@
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G74" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="H74" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>18</v>
@@ -3508,51 +3510,51 @@
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E76" s="6"/>
       <c r="F76" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G76" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="H76" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>34</v>
@@ -3562,16 +3564,16 @@
       </c>
       <c r="E77" s="6"/>
       <c r="F77" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G77" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="H77" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
variable defaults and help added more options to shiny
</commit_message>
<xml_diff>
--- a/inst/extdata/variable_defaults_and_help.xlsx
+++ b/inst/extdata/variable_defaults_and_help.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au530301_uni_au_dk/Documents/Vedhæftede filer/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{C2269CCF-9EE7-1446-93A5-54AE6600A477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AE4780C-1AC1-0945-9D93-A1154A22992A}"/>
+  <xr:revisionPtr revIDLastSave="333" documentId="8_{C2269CCF-9EE7-1446-93A5-54AE6600A477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8563FF1-012C-9A48-9D98-15709DB5BAF4}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="500" windowWidth="33680" windowHeight="19140" xr2:uid="{E0DFC8D9-2769-CD42-9190-B3351BDE6F8D}"/>
+    <workbookView xWindow="460" yWindow="500" windowWidth="35380" windowHeight="21900" xr2:uid="{E0DFC8D9-2769-CD42-9190-B3351BDE6F8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Shiny_Args" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Shiny_Args!$A$1:$J$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Shiny_Args!$A$1:$J$104</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="454">
   <si>
     <t>option_group</t>
   </si>
@@ -211,12 +211,6 @@
     <t>Reverse strand data represented as negative values</t>
   </si>
   <si>
-    <t>actual_strand_direction</t>
-  </si>
-  <si>
-    <t>true_strand</t>
-  </si>
-  <si>
     <t>Plot 5' left to 3' right</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t>log2transform</t>
   </si>
   <si>
-    <t>Log2-Transform Data</t>
-  </si>
-  <si>
     <t>Log2 transform the signal specific datasets. Pseudocount will automatically be added such that the lowest value in the dataset is 1, but it can also be assigned manually below.</t>
   </si>
   <si>
@@ -1012,9 +1003,6 @@
     <t>Height in centimeters of each sequencing track (full plot height will be influenced by this value). Options: positive numeric value. Recommended value between 0.2 and 1.0 cm.</t>
   </si>
   <si>
-    <t>off,no warnings,normal,detailed</t>
-  </si>
-  <si>
     <t>R_help</t>
   </si>
   <si>
@@ -1099,64 +1087,316 @@
     <t>0.5;10;1.2</t>
   </si>
   <si>
+    <t>10;1000;250</t>
+  </si>
+  <si>
+    <t>0;0.2;0.05</t>
+  </si>
+  <si>
+    <t>0.4;1.0;0.6</t>
+  </si>
+  <si>
+    <t>split_numeric</t>
+  </si>
+  <si>
+    <t>Upstream Extension;Downstream Extension</t>
+  </si>
+  <si>
+    <t>100,100;20,100;1</t>
+  </si>
+  <si>
+    <t>Horizontal line;Horizontal line2;Vertical line</t>
+  </si>
+  <si>
+    <t>1.00,1.00;0,100;0.025</t>
+  </si>
+  <si>
+    <t>split_text</t>
+  </si>
+  <si>
+    <t>Title color;Subtitle color;Scalebar color</t>
+  </si>
+  <si>
+    <t>0.5,1,0.5;0,5;0.25</t>
+  </si>
+  <si>
+    <t>0;1;0.2</t>
+  </si>
+  <si>
+    <t>4;18;6</t>
+  </si>
+  <si>
+    <t>Odd-numbered loci;Even-numbered loci</t>
+  </si>
+  <si>
+    <t>Horizontal separators;Vertical separators</t>
+  </si>
+  <si>
+    <t>Odd-numbered panels;Even-numbered panels</t>
+  </si>
+  <si>
+    <t>1;1000000;100</t>
+  </si>
+  <si>
+    <t>4;12;6</t>
+  </si>
+  <si>
+    <t>special_argument</t>
+  </si>
+  <si>
+    <t>4;18;7</t>
+  </si>
+  <si>
+    <t>First Panel Text Color;Inner Panels Text Color</t>
+  </si>
+  <si>
+    <t>4;18;9;6;6</t>
+  </si>
+  <si>
+    <t>optional_text</t>
+  </si>
+  <si>
+    <t>title of plot</t>
+  </si>
+  <si>
+    <t>1;1000000000;1</t>
+  </si>
+  <si>
+    <t>intermingled_color</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>same,complementary,analogous_right,analogous_left</t>
+  </si>
+  <si>
+    <t>intrmngld_col</t>
+  </si>
+  <si>
+    <t>Color Display of Data from Negative Strand</t>
+  </si>
+  <si>
+    <t>-1;1000000000;-1</t>
+  </si>
+  <si>
+    <t>Verbosity of information displayed in console.</t>
+  </si>
+  <si>
+    <t>Should a dummy plot (without sequencing data, for aestetic trials) be generated? This allows fast debugging of the "Plot Display Parameters".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify a scaling factor to apply for on-screen display ("Draw Plot") - ignored when exporting to pdf ('Save as Pdf'). </t>
+  </si>
+  <si>
+    <t>Specify a title to be used instead of the automatically generated title based on the name of the locus.</t>
+  </si>
+  <si>
+    <t>Should genomic scale be displayed?</t>
+  </si>
+  <si>
+    <t>Display genomic scale above tracks (otherwise it will be displayed below).</t>
+  </si>
+  <si>
+    <t>Percent opacity of the forward and reverse strand, respectively (100=full;0=blank). Default is 100 for both. Ignored if 'Enhance Signals' is selected under "Dataset-Specific Options".</t>
+  </si>
+  <si>
+    <t>Specify if reverse strand data should be represented as negative values. This is automatically the case with 'Intermingled Strands' display.</t>
+  </si>
+  <si>
+    <t>If data is only plotted for the strand of interest (i.e. "Display both strands" is deselected), reverse strand loci can be horizontally mirrored (5'-left to 3'-right). This option substantially slows down the plotting time.</t>
+  </si>
+  <si>
+    <t>When the "Intermingled strands display" option is selected, it may be beneficial to display data from the two strands with different colors. This can be done by changing the opacity and/or by choosing one of the options complementary, analogous_right and analogous_left.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra space up- and downstream of and relative to the selected genomic feature (0.1 = 10%). Only taken into account when genomic locus name is entered - ignored when genomic coordinates are entered. </t>
+  </si>
+  <si>
+    <t>Height in centimeters of each sequencing track (full plot height will be influenced by this value). Will be automatically determined if unselected. However, this requires that "Full Plot Height (cm)" is specified.</t>
+  </si>
+  <si>
+    <t>Specify the width in centimeters for the sequencing track window of the plot (full plot width will be influenced by this value).</t>
+  </si>
+  <si>
+    <t>Specify the width in centimeters of the margins on each side of the sequencing tracks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in cm allocated to the tracks scale. Ignored if "Display track scales" is deselected. Will be automatically determined if unselected (recommended). </t>
+  </si>
+  <si>
+    <t>Specify the plot height in centimeters. Will be automatically determined if unselected (recommended).</t>
+  </si>
+  <si>
+    <t>Specify the plot width in centimeters. Will be automatically determined if unselected (recommended).</t>
+  </si>
+  <si>
+    <t>Should scales of individual tracks be displayed (to the left of tracks)?</t>
+  </si>
+  <si>
+    <t>Calculate and display mean of replicates for specific datasets. If deselected, the individual replicates will be displayed.</t>
+  </si>
+  <si>
+    <t>Some bigwigs are deposited with negative values for minus strand coordinates. Select if this is true. Should be evaluated upfront by independent means (e.g. the IGV browser).</t>
+  </si>
+  <si>
+    <t>Specify whether the signal needs to be enhanced for specific datasets. This option may be useful to increase visibility for non-continuous/dispersed data such as e.g. 5'- and 3'-ends.</t>
+  </si>
+  <si>
+    <t>log2-Transform Data</t>
+  </si>
+  <si>
+    <t>log2 transform the signal from specific datasets. Pseudocount will automatically be added such that the lowest "pre-transformation" value in the dataset is 1 (tranformed value of 0), but it can also be assigned manually below.</t>
+  </si>
+  <si>
+    <t>Set negative values in specific datasets to 0. If the data is of a type where background signal is subtracted, negative values can be set to 0.</t>
+  </si>
+  <si>
+    <t>split_color</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Forward Tracks Opacity (%);Reverse Tracks Opacity (%)</t>
+  </si>
+  <si>
+    <t>Height in centimeters of the title field (full plot height will be influenced by this value).</t>
+  </si>
+  <si>
+    <t>Height in centimeters of the genomic scale field (full plot height will be influenced by this value).</t>
+  </si>
+  <si>
+    <t>Height in centimeters of each line in the annotation track (full plot height will be influenced by this value).</t>
+  </si>
+  <si>
+    <t>Height in centimeters of each spacer line used in the plot (full plot height will be influenced by this value).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum width in cm that can be occupied by the “sample information” panel (to the left of tracks). Text truncation may occur if the value makes the panel too narrow. Will be automatically determined if unselected (recommended). </t>
+  </si>
+  <si>
+    <t>Specify the desired binning method – which summary statistic should be used on the signal within each bin (mean, median or max).</t>
+  </si>
+  <si>
+    <t>Specify if batch correction should be used for your dataset(s) of interest. Batch correction is based on the limma package and is conducted on the log2-transformed signal in individual bins, and can be conducted based on the full dataset, while only plotting a subset. If "log2-Transform Data" is not selected, the signal will be back-transformed (anti-log2).</t>
+  </si>
+  <si>
+    <t>Specify if the tracks labels should mandatorily occupy all the space provided under "Plot Display Parameters::Panels Width (cm)" or if they can use less should it be possible. Ignored if "Panels Width (cm)" is deselected, which means that the combined width of the panels will be automatically determined.</t>
+  </si>
+  <si>
+    <t>If deselected, an automatic assignment based on available space will be performed. If selected, subsequently select which dataset and/or subgroup panels text should be displayed horizontally (if deselected they will be displayed vertically).</t>
+  </si>
+  <si>
+    <t>Color(s) of the panel text (can be entered manually as name or hex code).</t>
+  </si>
+  <si>
+    <t>Font size(s) for panel text. Will be automatically assigned when deselected.</t>
+  </si>
+  <si>
+    <t>Font sizes for each dataset and subgroup. Will be automatically assigned when deselected.</t>
+  </si>
+  <si>
+    <t>Should the left-most panels, which displays dataset names, be displayed? Can e.g. be omitted if all datasets consist of only one sample or if all samples are contained within one dataset.</t>
+  </si>
+  <si>
+    <t>Specify if a white space should be inserted between sequencing datasets tracks. The separation between datasets can be further enhanced by selecting "Horizontal separators" below.</t>
+  </si>
+  <si>
+    <t>Specify if horizontal and/or vertical line-separators should be displayed in order to clearly separate panels. Horizontal line-separators will only be displayed if 'Dataset Spacers' is selected.</t>
+  </si>
+  <si>
+    <t>Color(s) of the separators (can be entered manually as name or hex code). "Horizontal line", "Horizontal line2" and "Vertictal line" correspond to 'line-spacer', 'thickline-spacer' and 'vertical-spacer' in the "Plot Layout::Plotting Segment Order".</t>
+  </si>
+  <si>
+    <t>Weight of the separators. "Horizontal line", "Horizontal line2" and "Vertictal line" correspond to 'line-spacer', 'thickline-spacer' and 'vertical-spacer' in the "Plot Layout::Plotting Segment Order".</t>
+  </si>
+  <si>
+    <t>Should the background of the tracks alternate between datasets for easier discrimination? Colors to use can be specified below. If deselected there will be no background color.</t>
+  </si>
+  <si>
+    <t>Background colors (can be entered manually as name or hex code).</t>
+  </si>
+  <si>
+    <t>Background color opacity.</t>
+  </si>
+  <si>
+    <t>Deselected per default, which means that the bin size will be automatically determined. If selected, the bin size can be entered as a positive integer value. The lower the value, the slower the plotting.</t>
+  </si>
+  <si>
+    <t>Center the bins around the given genomic position. Provide an integer value that lies within the plotted region. Deselected per default, which means that the bin center will be at the 5'-end of the plotted region if it is defined by genomic coordinates and at the 5'-end of the locus if the plotted region is defined by locus name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Font colors of the header region – Title, Subtitle (=genomic range) and Scalebar (can be entered manually as name or hex code). </t>
+  </si>
+  <si>
+    <t>Font size of the genomic scale can be automatically (deselected) or manually (selected) determined.</t>
+  </si>
+  <si>
+    <t>Font sizes in the header region – Title, Subtitle (=genomic range) and Scalebar – can be automatically (deselected) or manually (selected) determined.</t>
+  </si>
+  <si>
+    <t>For each dataset, specify whether to "group" auto-scale or just auto-scale for each individual track.</t>
+  </si>
+  <si>
+    <t>The scale can be set manually for individual datasets (and for the forward and reverse strand). Provide the maximum value for the data scale (y-axis) for each dataset. -1 leads to auto-scaling.</t>
+  </si>
+  <si>
+    <t>Should scientific number format be used for the tracks scale.</t>
+  </si>
+  <si>
+    <t>Shading color opacity.</t>
+  </si>
+  <si>
+    <t>Shading colors (can be entered manually as name or hex code).</t>
+  </si>
+  <si>
+    <t>Color of the data scales and font (can be entered manually as name or hex code).</t>
+  </si>
+  <si>
+    <t>Color of the genomic scale and font (can be entered manually as name or hex code).</t>
+  </si>
+  <si>
+    <t>Individual loci within the plotted region can be highlighted with a shaded box of alternating colors (specified below). This may help distinguish the different loci within the plotted region.</t>
+  </si>
+  <si>
+    <t>Color of the titles of the annotation(s) depicted in the left panel (can be entered manually as name or hex code).</t>
+  </si>
+  <si>
+    <t>Text color of the annotated feature name (can be entered manually as name or hex code).</t>
+  </si>
+  <si>
+    <t>Set the annotation packing for each annotation. 'expanded' and 'squished' display the detailed structures of transcripts under a given feature either as fully expanded or squished. ’collapsed’ collapses all overlapping features into one 'super-exon' feature whereas 'collapsed2’ only collapses features belonging to the same locus into one 'super-exon' feature.</t>
+  </si>
+  <si>
+    <t>Display locus/feature names in the annotation panel.</t>
+  </si>
+  <si>
+    <t>Locus/feature names will be centered based on the the transcript density within a given locus rather than the center. Probably only makes sense if there is a very long outlier transcript that moves the center away from the major transcript variants.</t>
+  </si>
+  <si>
+    <t>If selected, feature names are displayed above features. If deselected, feature names are displayed below features.</t>
+  </si>
+  <si>
+    <t>Display reverse strand features as a miror of the forward strand, which is determined by selecting/deselecting the above tickbox 'Feature Names Above Features'. Will be ignored with "Plot layout::Intermingled strands display"</t>
+  </si>
+  <si>
+    <t>Color(s) used to visualize the annotated features (can be entered manually as name or hex code). If set to "white", the colors specified in the bed file will be used.</t>
+  </si>
+  <si>
     <t>0;10;1</t>
   </si>
   <si>
-    <t>10;1000;250</t>
-  </si>
-  <si>
-    <t>0;0.2;0.05</t>
-  </si>
-  <si>
-    <t>0.4;1.0;0.6</t>
-  </si>
-  <si>
-    <t>split_numeric</t>
-  </si>
-  <si>
-    <t>Forward Track Opacity;Reverse Track Opacity</t>
-  </si>
-  <si>
-    <t>Upstream Extension;Downstream Extension</t>
-  </si>
-  <si>
-    <t>100,100;20,100;1</t>
-  </si>
-  <si>
-    <t>Horizontal line;Horizontal line2;Vertical line</t>
-  </si>
-  <si>
-    <t>1.00,1.00;0,100;0.025</t>
-  </si>
-  <si>
-    <t>split_text</t>
-  </si>
-  <si>
-    <t>Title color;Subtitle color;Scalebar color</t>
-  </si>
-  <si>
-    <t>0.5,1,0.5;0,5;0.25</t>
-  </si>
-  <si>
-    <t>0;1;0.2</t>
-  </si>
-  <si>
-    <t>4;18;9</t>
-  </si>
-  <si>
-    <t>4;18;6</t>
-  </si>
-  <si>
-    <t>Odd-numbered loci;Even-numbered loci</t>
-  </si>
-  <si>
-    <t>Horizontal separators;Vertical separators</t>
-  </si>
-  <si>
-    <t>First Panel Text Color;Other Panels Text Color</t>
-  </si>
-  <si>
-    <t>Odd-numbered panels;Even-numbered panels</t>
+    <t>Add pseudocount to values in specific datasets to allow log2-transformation. The lowest "pre-transformation" value in the dataset should be ≥ 1 (tranformed value of ≥ 0) – assigned pseudocount values [0;1[ that do fulfill this rule will be auto-corrected.</t>
+  </si>
+  <si>
+    <t>off,no warnings,normal,detailed</t>
+  </si>
+  <si>
+    <t>reverse_strand_direction</t>
+  </si>
+  <si>
+    <t>reverse_strand</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1425,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1210,18 +1450,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1235,7 +1463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1285,10 +1513,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1606,20 +1837,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE4A534-F197-8749-AB2A-361DC1DBAF63}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="98" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="30.5" customWidth="1"/>
+    <col min="5" max="6" width="30.5" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="67.5" customWidth="1"/>
     <col min="9" max="10" width="124.5" customWidth="1"/>
@@ -1655,10 +1885,10 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1672,7 +1902,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>325</v>
+        <v>451</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>13</v>
@@ -1684,7 +1914,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>15</v>
+        <v>381</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>15</v>
@@ -1714,7 +1944,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>21</v>
+        <v>382</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>21</v>
@@ -1734,7 +1964,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>18</v>
@@ -1746,7 +1976,7 @@
         <v>26</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>27</v>
+        <v>383</v>
       </c>
       <c r="J4" s="15" t="s">
         <v>27</v>
@@ -1790,12 +2020,14 @@
         <v>32</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>33</v>
+        <v>372</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>373</v>
+      </c>
       <c r="F6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1806,7 +2038,7 @@
         <v>36</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>37</v>
+        <v>384</v>
       </c>
       <c r="J6" s="15" t="s">
         <v>37</v>
@@ -1836,7 +2068,7 @@
         <v>39</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>40</v>
+        <v>385</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>40</v>
@@ -1866,13 +2098,13 @@
         <v>42</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>43</v>
+        <v>386</v>
       </c>
       <c r="J8" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1880,13 +2112,13 @@
         <v>44</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>359</v>
+        <v>407</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>18</v>
@@ -1898,48 +2130,48 @@
         <v>46</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>327</v>
+        <v>387</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>47</v>
+        <v>375</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>377</v>
+      </c>
       <c r="F10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>48</v>
+        <v>378</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>49</v>
+        <v>379</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>50</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>17</v>
@@ -1952,16 +2184,16 @@
         <v>18</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1969,7 +2201,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>17</v>
@@ -1982,46 +2214,46 @@
         <v>18</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>328</v>
+        <v>54</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>329</v>
+        <v>388</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2029,29 +2261,29 @@
         <v>9</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>61</v>
+        <v>452</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="D14" s="9" t="b">
+        <v>0</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>62</v>
+        <v>453</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>64</v>
+        <v>389</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>64</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2059,7 +2291,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>33</v>
@@ -2072,48 +2304,46 @@
         <v>18</v>
       </c>
       <c r="G15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>73</v>
+      <c r="J16" s="15" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2121,127 +2351,127 @@
         <v>9</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="I18" s="14" t="s">
-        <v>323</v>
+        <v>392</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>80</v>
+      <c r="B19" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>80</v>
+        <v>68</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>83</v>
+      <c r="B20" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2249,31 +2479,31 @@
         <v>9</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D21" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>347</v>
-      </c>
       <c r="F21" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>90</v>
+        <v>83</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>410</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2281,31 +2511,31 @@
         <v>9</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="D22" s="9">
-        <v>12</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>351</v>
-      </c>
       <c r="F22" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2313,93 +2543,95 @@
         <v>9</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D23" s="9">
+        <v>12</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="H24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="I24" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="J24" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="8" t="s">
+    </row>
+    <row r="25" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="C25" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="J23" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="8" t="s">
+      <c r="E25" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="H25" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>106</v>
-      </c>
       <c r="I25" s="14" t="s">
-        <v>107</v>
+        <v>412</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>107</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2407,31 +2639,29 @@
         <v>9</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>357</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D26" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3"/>
       <c r="F26" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>111</v>
+        <v>398</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2439,31 +2669,31 @@
         <v>9</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>115</v>
+        <v>395</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2471,161 +2701,163 @@
         <v>9</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G28" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="J29" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="H28" s="8" t="s">
+    </row>
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="B30" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="J30" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="G31" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="9" t="s">
+      <c r="F32" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="H32" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G31" s="8" t="s">
+      <c r="I32" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="J32" s="15" t="s">
         <v>131</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>17</v>
@@ -2635,89 +2867,89 @@
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G33" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="C35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H35" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="I35" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="J35" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="J33" s="15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="17" t="s">
+    </row>
+    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="9">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>17</v>
@@ -2727,27 +2959,27 @@
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>150</v>
+        <v>404</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>17</v>
@@ -2756,28 +2988,28 @@
         <v>0</v>
       </c>
       <c r="E37" s="3"/>
-      <c r="F37" s="6" t="s">
-        <v>152</v>
+      <c r="F37" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="J37" s="14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>17</v>
@@ -2787,49 +3019,49 @@
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="J38" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="J38" s="14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="4"/>
+        <v>368</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="3"/>
       <c r="F39" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>163</v>
+        <v>416</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2837,7 +3069,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>17</v>
@@ -2847,179 +3079,183 @@
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J40" s="14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="D41" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G41" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="E43" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="I41" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="J41" s="14" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="8" t="s">
+      <c r="H43" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="I43" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="J43" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G42" s="8" t="s">
+    </row>
+    <row r="44" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="H42" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="J42" s="14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="J43" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>179</v>
-      </c>
       <c r="C44" s="8" t="s">
-        <v>33</v>
+        <v>368</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>369</v>
+      </c>
       <c r="F44" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G44" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="J44" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="I45" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="J45" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>17</v>
@@ -3029,239 +3265,239 @@
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G46" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="C48" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D48" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="I46" s="14" t="s">
+      <c r="E48" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="J46" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="H48" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="D47" s="9" t="s">
+      <c r="C49" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G47" s="8" t="s">
+      <c r="E49" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="H47" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="I47" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="J47" s="14" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="H49" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="D48" s="10" t="s">
+      <c r="I49" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="J49" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G48" s="8" t="s">
+    </row>
+    <row r="50" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="C50" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="I48" s="14" t="s">
+      <c r="H50" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="J48" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" s="8" t="s">
+      <c r="I50" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="J50" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G49" s="8" t="s">
+    </row>
+    <row r="51" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="C51" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="I49" s="14" t="s">
+      <c r="H51" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="J49" s="14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B50" s="18" t="s">
+      <c r="I51" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="J51" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G50" s="8" t="s">
+    </row>
+    <row r="52" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="H50" s="8" t="s">
+      <c r="C52" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D52" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="I50" s="14" t="s">
+      <c r="E52" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G52" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="J50" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B51" s="18" t="s">
+      <c r="H52" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="D51" s="10" t="s">
+      <c r="I52" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="J52" s="14" t="s">
         <v>207</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I51" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="J51" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="I52" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="J52" s="14" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>216</v>
+      <c r="B53" s="17" t="s">
+        <v>208</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="7" t="s">
-        <v>217</v>
+        <v>23</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="J53" s="15" t="s">
-        <v>333</v>
+        <v>211</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="J53" s="14" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3269,279 +3505,283 @@
         <v>9</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="I54" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="J54" s="15" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="J55" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="9" t="s">
+    </row>
+    <row r="56" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="9">
+        <v>250</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="I56" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="J56" s="15" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="D57" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="I54" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="J54" s="15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D55" s="9">
-        <v>250</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="G55" s="8" t="s">
+      <c r="E57" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="G57" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="I55" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="J55" s="15" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" s="18" t="s">
+      <c r="H57" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="F56" s="6" t="s">
+      <c r="C58" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="E58" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G58" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="H56" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="I56" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="J56" s="14" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B57" s="8" t="s">
+      <c r="H58" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="I58" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="J58" s="14" t="s">
         <v>230</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="I57" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="J57" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E58" s="3"/>
-      <c r="F58" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="I58" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="J58" s="14" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="8" t="s">
-        <v>238</v>
+      <c r="B59" s="17" t="s">
+        <v>231</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>343</v>
+        <v>406</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>369</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E59" s="3"/>
       <c r="F59" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>334</v>
+        <v>233</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>337</v>
+        <v>439</v>
       </c>
       <c r="J59" s="14" t="s">
-        <v>337</v>
+        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>320</v>
+        <v>235</v>
       </c>
       <c r="C60" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="I60" s="14" t="s">
+        <v>431</v>
+      </c>
+      <c r="J60" s="14" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="9" t="b">
+      <c r="D61" s="9" t="b">
         <v>1</v>
-      </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="H60" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="I60" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="J60" s="15" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="I61" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="J61" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="I62" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="J62" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="H61" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="I61" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="J61" s="15" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="I62" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="J62" s="15" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3549,159 +3789,163 @@
         <v>9</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>33</v>
+        <v>242</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="E63" s="4"/>
+        <v>243</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>335</v>
+      </c>
       <c r="F63" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>254</v>
+        <v>435</v>
       </c>
       <c r="J63" s="15" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E64" s="4"/>
+      <c r="F64" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="I64" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="J64" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="I65" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="C64" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="G64" s="8" t="s">
+      <c r="J65" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="H64" s="8" t="s">
+      <c r="B66" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="I64" s="15" t="s">
+      <c r="C66" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="J64" s="15" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
+      <c r="E66" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="F66" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" s="10" t="s">
+      <c r="G66" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="H66" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="I66" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="J66" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="G65" s="8" t="s">
+    </row>
+    <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="H65" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="J65" s="14" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D66" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G66" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="H66" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="I66" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="J66" s="14" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A67" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>271</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D67" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>274</v>
+        <v>444</v>
       </c>
       <c r="J67" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>259</v>
+        <v>9</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>17</v>
@@ -3711,57 +3955,57 @@
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>278</v>
+        <v>445</v>
       </c>
       <c r="J68" s="14" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>9</v>
+        <v>256</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D69" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>340</v>
+        <v>446</v>
       </c>
       <c r="J69" s="14" t="s">
-        <v>340</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>259</v>
+        <v>9</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>17</v>
@@ -3771,273 +4015,303 @@
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>285</v>
+        <v>447</v>
       </c>
       <c r="J70" s="14" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B71" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E72" s="5"/>
+      <c r="F72" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="H72" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="J72" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D71" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E71" s="5"/>
-      <c r="F71" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="I71" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="J71" s="14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="H72" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="I72" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="J72" s="14" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>294</v>
+      <c r="B73" s="17" t="s">
+        <v>287</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>343</v>
+        <v>406</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>352</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E73" s="3"/>
       <c r="F73" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>297</v>
+        <v>442</v>
       </c>
       <c r="J73" s="14" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="12" t="s">
-        <v>298</v>
+      <c r="B74" s="8" t="s">
+        <v>291</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D74" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="E74" s="4"/>
+        <v>339</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>348</v>
+      </c>
       <c r="F74" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="J74" s="14" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="E75" s="4"/>
+      <c r="F75" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="H75" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="I75" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="J75" s="14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="H76" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="I76" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="C75" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G75" s="8" t="s">
+      <c r="J76" s="14" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="H75" s="8" t="s">
+      <c r="C77" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G77" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="I75" s="14" t="s">
+      <c r="H77" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="J75" s="14" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A76" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="B76" s="8" t="s">
+      <c r="I77" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="J77" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="C76" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="3"/>
-      <c r="F76" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G76" s="8" t="s">
+    </row>
+    <row r="78" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="H76" s="8" t="s">
+      <c r="C78" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D78" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="I76" s="14" t="s">
+      <c r="E78" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G78" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="J76" s="14" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B77" s="8" t="s">
+      <c r="H78" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="C77" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="D77" s="10" t="s">
+      <c r="I78" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="J78" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G77" s="8" t="s">
+    </row>
+    <row r="79" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="H77" s="8" t="s">
+      <c r="C79" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="H79" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="I77" s="14" t="s">
+      <c r="I79" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="J79" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="J77" s="14" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="H78" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="I78" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="J78" s="14" t="s">
-        <v>318</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J103" xr:uid="{1BE4A534-F197-8749-AB2A-361DC1DBAF63}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J103">
-      <sortCondition ref="F1:F103"/>
+  <autoFilter ref="A1:J104" xr:uid="{1BE4A534-F197-8749-AB2A-361DC1DBAF63}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J104">
+      <sortCondition ref="F1:F104"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Fixed bugs related to conversion of NULL, TRUE, FALSE and NA from character to boolean in shinyApp
</commit_message>
<xml_diff>
--- a/inst/extdata/variable_defaults_and_help.xlsx
+++ b/inst/extdata/variable_defaults_and_help.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au103725/Library/CloudStorage/OneDrive-AarhusUniversitet/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E78840-F01E-FA4F-A25E-EB29681773CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF88E2D-3A15-7648-8824-109224AB0F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{E0DFC8D9-2769-CD42-9190-B3351BDE6F8D}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="459">
   <si>
     <t>option_group</t>
   </si>
@@ -1402,6 +1402,9 @@
   </si>
   <si>
     <t>XX</t>
+  </si>
+  <si>
+    <t>annot_height_cm</t>
   </si>
 </sst>
 </file>
@@ -1858,7 +1861,7 @@
   <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2542,7 +2545,7 @@
         <v>68</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>81</v>
+        <v>458</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
Center of bins bug fixed
</commit_message>
<xml_diff>
--- a/inst/extdata/variable_defaults_and_help.xlsx
+++ b/inst/extdata/variable_defaults_and_help.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au103725/Library/CloudStorage/OneDrive-AarhusUniversitet/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF88E2D-3A15-7648-8824-109224AB0F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7054CB0D-7E91-914A-8F31-7659129EFC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{E0DFC8D9-2769-CD42-9190-B3351BDE6F8D}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="98" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Annotation bug fix + tool tips
</commit_message>
<xml_diff>
--- a/inst/extdata/variable_defaults_and_help.xlsx
+++ b/inst/extdata/variable_defaults_and_help.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au103725/Library/CloudStorage/OneDrive-AarhusUniversitet/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724835E1-0316-4349-8C8B-49D0BDBB4C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2632DE5B-BDED-F24B-BD1B-D856A07E0611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{E0DFC8D9-2769-CD42-9190-B3351BDE6F8D}"/>
   </bookViews>
@@ -987,9 +987,6 @@
     <t>For each dataset, specify whether to 'group' auto-scale or just auto-scale for each individual track.</t>
   </si>
   <si>
-    <t>Height in centimeters of the title field (full plot height will be influenced based on this value). Options: positive numeric value.</t>
-  </si>
-  <si>
     <t>Height in centimeters of each sequencing track (full plot height will be influenced by this value). Options: positive numeric value. Recommended value between 0.2 and 1.0 cm.</t>
   </si>
   <si>
@@ -1251,9 +1248,6 @@
     <t>Forward Tracks Opacity (%);Reverse Tracks Opacity (%)</t>
   </si>
   <si>
-    <t>Height in centimeters of the title field (full plot height will be influenced by this value).</t>
-  </si>
-  <si>
     <t>Height in centimeters of the genomic scale field (full plot height will be influenced by this value).</t>
   </si>
   <si>
@@ -1398,20 +1392,26 @@
     <t>Track Colors</t>
   </si>
   <si>
-    <t>XX</t>
-  </si>
-  <si>
     <t>annot_height_cm</t>
   </si>
   <si>
     <t>Specify the order of displayed vertical segments in the plot using the following segment-labels:header, scale, names of individual datasets, annotations, unstranded-beds, thickline-spacer, line-spacer and empty-spacer. There should be perfect correspondance between datasets to display and the listed datasets.</t>
+  </si>
+  <si>
+    <t>Height in centimeters of the title field (full plot height will be influenced by this value). Will be ignored if the field is set too small to fit the font size selected for the title.</t>
+  </si>
+  <si>
+    <t>Height in centimeters of the title field (full plot height will be influenced based on this value). Options: positive numeric value. Will be ignored if the field is set too small to fit the font size selected for the title.</t>
+  </si>
+  <si>
+    <t>Pick colors for the individual sample tracks (replicates for a given sample will get the same color).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1428,13 +1428,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1531,16 +1524,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1860,8 +1853,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1906,7 +1899,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1923,7 +1916,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>13</v>
@@ -1935,7 +1928,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>15</v>
@@ -1946,29 +1939,29 @@
         <v>117</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>190</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="21" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1995,7 +1988,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J4" s="15" t="s">
         <v>21</v>
@@ -2015,7 +2008,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>18</v>
@@ -2027,7 +2020,7 @@
         <v>26</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J5" s="15" t="s">
         <v>27</v>
@@ -2071,13 +2064,13 @@
         <v>32</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>18</v>
@@ -2089,7 +2082,7 @@
         <v>36</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>37</v>
@@ -2119,7 +2112,7 @@
         <v>39</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J8" s="15" t="s">
         <v>40</v>
@@ -2149,7 +2142,7 @@
         <v>42</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J9" s="15" t="s">
         <v>43</v>
@@ -2163,13 +2156,13 @@
         <v>44</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>18</v>
@@ -2181,10 +2174,10 @@
         <v>46</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2192,28 +2185,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>375</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>376</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>378</v>
-      </c>
       <c r="I11" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J11" s="15"/>
     </row>
@@ -2301,10 +2294,10 @@
         <v>57</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2312,7 +2305,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>17</v>
@@ -2325,16 +2318,16 @@
         <v>18</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>58</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -2361,10 +2354,10 @@
         <v>61</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2405,13 +2398,13 @@
         <v>66</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>353</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>67</v>
@@ -2423,7 +2416,7 @@
         <v>69</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J18" s="14" t="s">
         <v>70</v>
@@ -2437,13 +2430,13 @@
         <v>71</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D19" s="9">
         <v>0.3</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>67</v>
@@ -2455,13 +2448,13 @@
         <v>73</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>9</v>
       </c>
@@ -2469,13 +2462,13 @@
         <v>74</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>67</v>
@@ -2487,10 +2480,10 @@
         <v>76</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>407</v>
+        <v>456</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>319</v>
+        <v>457</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2501,13 +2494,13 @@
         <v>77</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>81</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>67</v>
@@ -2519,7 +2512,7 @@
         <v>78</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="J21" s="16" t="s">
         <v>79</v>
@@ -2533,25 +2526,25 @@
         <v>80</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>67</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>82</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="J22" s="14" t="s">
         <v>83</v>
@@ -2565,13 +2558,13 @@
         <v>84</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>67</v>
@@ -2583,7 +2576,7 @@
         <v>86</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J23" s="16" t="s">
         <v>87</v>
@@ -2597,13 +2590,13 @@
         <v>88</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D24" s="9">
         <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>67</v>
@@ -2615,7 +2608,7 @@
         <v>90</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J24" s="14" t="s">
         <v>91</v>
@@ -2635,7 +2628,7 @@
         <v>93</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>67</v>
@@ -2647,7 +2640,7 @@
         <v>95</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J25" s="14" t="s">
         <v>96</v>
@@ -2661,13 +2654,13 @@
         <v>97</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>98</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>67</v>
@@ -2679,10 +2672,10 @@
         <v>100</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2709,7 +2702,7 @@
         <v>103</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J27" s="14" t="s">
         <v>104</v>
@@ -2723,13 +2716,13 @@
         <v>105</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>67</v>
@@ -2741,7 +2734,7 @@
         <v>107</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>108</v>
@@ -2755,13 +2748,13 @@
         <v>109</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>67</v>
@@ -2773,7 +2766,7 @@
         <v>111</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>112</v>
@@ -2787,13 +2780,13 @@
         <v>113</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>67</v>
@@ -2805,7 +2798,7 @@
         <v>115</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>116</v>
@@ -2835,7 +2828,7 @@
         <v>120</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J31" s="15" t="s">
         <v>121</v>
@@ -2865,7 +2858,7 @@
         <v>123</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>124</v>
@@ -2897,7 +2890,7 @@
         <v>129</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="J33" s="15" t="s">
         <v>130</v>
@@ -2927,7 +2920,7 @@
         <v>133</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J34" s="15" t="s">
         <v>134</v>
@@ -2954,10 +2947,10 @@
         <v>135</v>
       </c>
       <c r="H35" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="I35" s="15" t="s">
         <v>401</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>402</v>
       </c>
       <c r="J35" s="15" t="s">
         <v>136</v>
@@ -2977,7 +2970,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>119</v>
@@ -2989,7 +2982,7 @@
         <v>138</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>139</v>
@@ -3019,7 +3012,7 @@
         <v>141</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J37" s="15" t="s">
         <v>142</v>
@@ -3049,7 +3042,7 @@
         <v>145</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J38" s="15" t="s">
         <v>146</v>
@@ -3079,7 +3072,7 @@
         <v>150</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>151</v>
@@ -3093,7 +3086,7 @@
         <v>152</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>34</v>
@@ -3109,7 +3102,7 @@
         <v>154</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J40" s="14" t="s">
         <v>155</v>
@@ -3199,10 +3192,10 @@
         <v>165</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3213,13 +3206,13 @@
         <v>166</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>167</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>148</v>
@@ -3231,7 +3224,7 @@
         <v>169</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J44" s="14" t="s">
         <v>170</v>
@@ -3245,13 +3238,13 @@
         <v>171</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>148</v>
@@ -3263,7 +3256,7 @@
         <v>173</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J45" s="14" t="s">
         <v>174</v>
@@ -3277,13 +3270,13 @@
         <v>175</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>148</v>
@@ -3295,7 +3288,7 @@
         <v>177</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J46" s="14" t="s">
         <v>178</v>
@@ -3325,7 +3318,7 @@
         <v>180</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="J47" s="14" t="s">
         <v>181</v>
@@ -3355,7 +3348,7 @@
         <v>184</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J48" s="14" t="s">
         <v>185</v>
@@ -3369,13 +3362,13 @@
         <v>186</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>187</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>148</v>
@@ -3387,10 +3380,10 @@
         <v>315</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3401,13 +3394,13 @@
         <v>189</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>190</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>148</v>
@@ -3419,7 +3412,7 @@
         <v>192</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J50" s="14" t="s">
         <v>193</v>
@@ -3433,13 +3426,13 @@
         <v>194</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>148</v>
@@ -3451,7 +3444,7 @@
         <v>196</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="J51" s="14" t="s">
         <v>197</v>
@@ -3481,7 +3474,7 @@
         <v>200</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J52" s="14" t="s">
         <v>201</v>
@@ -3495,13 +3488,13 @@
         <v>202</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>203</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>148</v>
@@ -3513,7 +3506,7 @@
         <v>205</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J53" s="14" t="s">
         <v>206</v>
@@ -3533,7 +3526,7 @@
         <v>208</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>148</v>
@@ -3545,7 +3538,7 @@
         <v>210</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J54" s="14" t="s">
         <v>211</v>
@@ -3559,13 +3552,13 @@
         <v>212</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>213</v>
@@ -3577,10 +3570,10 @@
         <v>215</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J55" s="15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -3591,13 +3584,13 @@
         <v>216</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>213</v>
@@ -3609,7 +3602,7 @@
         <v>218</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="J56" s="15" t="s">
         <v>219</v>
@@ -3629,7 +3622,7 @@
         <v>250</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>213</v>
@@ -3641,10 +3634,10 @@
         <v>222</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J57" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3655,13 +3648,13 @@
         <v>223</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>224</v>
@@ -3670,13 +3663,13 @@
         <v>225</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J58" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3687,13 +3680,13 @@
         <v>226</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>227</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>224</v>
@@ -3702,10 +3695,10 @@
         <v>228</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J59" s="14" t="s">
         <v>229</v>
@@ -3719,7 +3712,7 @@
         <v>230</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>190</v>
@@ -3735,7 +3728,7 @@
         <v>232</v>
       </c>
       <c r="I60" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J60" s="14" t="s">
         <v>233</v>
@@ -3749,13 +3742,13 @@
         <v>234</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>224</v>
@@ -3764,13 +3757,13 @@
         <v>235</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I61" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J61" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3797,7 +3790,7 @@
         <v>317</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="J62" s="15" t="s">
         <v>318</v>
@@ -3811,13 +3804,13 @@
         <v>236</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>237</v>
@@ -3829,7 +3822,7 @@
         <v>239</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J63" s="15" t="s">
         <v>240</v>
@@ -3849,7 +3842,7 @@
         <v>242</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>237</v>
@@ -3861,7 +3854,7 @@
         <v>244</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="J64" s="15" t="s">
         <v>245</v>
@@ -3875,7 +3868,7 @@
         <v>246</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>247</v>
@@ -3891,7 +3884,7 @@
         <v>249</v>
       </c>
       <c r="I65" s="15" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J65" s="15" t="s">
         <v>250</v>
@@ -3905,13 +3898,13 @@
         <v>251</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>237</v>
@@ -3955,7 +3948,7 @@
         <v>261</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J67" s="14" t="s">
         <v>262</v>
@@ -3985,7 +3978,7 @@
         <v>265</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J68" s="14" t="s">
         <v>266</v>
@@ -4015,7 +4008,7 @@
         <v>269</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J69" s="14" t="s">
         <v>270</v>
@@ -4045,7 +4038,7 @@
         <v>273</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J70" s="14" t="s">
         <v>274</v>
@@ -4075,10 +4068,10 @@
         <v>277</v>
       </c>
       <c r="I71" s="14" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="J71" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -4119,7 +4112,7 @@
         <v>282</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D73" s="11" t="s">
         <v>190</v>
@@ -4135,7 +4128,7 @@
         <v>284</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J73" s="14" t="s">
         <v>285</v>
@@ -4149,7 +4142,7 @@
         <v>286</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>190</v>
@@ -4165,7 +4158,7 @@
         <v>288</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J74" s="14" t="s">
         <v>289</v>
@@ -4179,13 +4172,13 @@
         <v>290</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>259</v>
@@ -4211,7 +4204,7 @@
         <v>294</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>295</v>
@@ -4227,7 +4220,7 @@
         <v>297</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J76" s="14" t="s">
         <v>298</v>
@@ -4241,13 +4234,13 @@
         <v>299</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>259</v>
@@ -4289,7 +4282,7 @@
         <v>305</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J78" s="14" t="s">
         <v>306</v>
@@ -4303,13 +4296,13 @@
         <v>307</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>308</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>259</v>
@@ -4321,7 +4314,7 @@
         <v>310</v>
       </c>
       <c r="I79" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="J79" s="14" t="s">
         <v>311</v>
@@ -4341,7 +4334,7 @@
         <v>93</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>259</v>
@@ -4353,7 +4346,7 @@
         <v>313</v>
       </c>
       <c r="I80" s="14" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J80" s="14" t="s">
         <v>314</v>

</xml_diff>

<commit_message>
squished annotation bug fix
</commit_message>
<xml_diff>
--- a/inst/extdata/variable_defaults_and_help.xlsx
+++ b/inst/extdata/variable_defaults_and_help.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au103725/Library/CloudStorage/OneDrive-AarhusUniversitet/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2632DE5B-BDED-F24B-BD1B-D856A07E0611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095E6072-6247-0A49-A1D3-5527680E3DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{E0DFC8D9-2769-CD42-9190-B3351BDE6F8D}"/>
   </bookViews>
@@ -1471,7 +1471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1523,18 +1523,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1853,8 +1841,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1935,26 +1923,26 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="8" t="s">
         <v>453</v>
       </c>
       <c r="I3" s="14" t="s">

</xml_diff>

<commit_message>
roxygen2 @param added to seqNdisplay function
</commit_message>
<xml_diff>
--- a/inst/extdata/variable_defaults_and_help.xlsx
+++ b/inst/extdata/variable_defaults_and_help.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au530301_uni_au_dk/Documents/Vedhæftede filer/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{095E6072-6247-0A49-A1D3-5527680E3DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B16CBE43-54D2-5E4B-A971-B36A53BA1836}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{095E6072-6247-0A49-A1D3-5527680E3DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33198BD6-9D38-884A-ADBE-79E13EE6AE97}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{E0DFC8D9-2769-CD42-9190-B3351BDE6F8D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="462">
   <si>
     <t>option_group</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Scaling For On-Screen Display</t>
   </si>
   <si>
-    <t xml:space="preserve">Specify a scaling factor to apply for on-screen display ('Draw Plot') - ignored when exporting to pdf ('Save as Pdf'). </t>
-  </si>
-  <si>
     <t>suppress_header</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Specify a title to be used instead of the automatically generated title based on the name of the locus. If genomic coordinates are used, the title panel will be excluded per default unless specified here.</t>
-  </si>
-  <si>
     <t>include_genomic_scale</t>
   </si>
   <si>
@@ -250,9 +244,6 @@
     <t>Expand Plotted Region (Upstream/Downstream)</t>
   </si>
   <si>
-    <t xml:space="preserve">Extra space up- and downstream of and relative to the selected genomic feature (0.1 = 10%). Only taken into account when genomic locus name is entered - ignored when genomic coordinates are entered.  Comma separated 1.5,1.5. </t>
-  </si>
-  <si>
     <t>track_height_cm</t>
   </si>
   <si>
@@ -271,9 +262,6 @@
     <t>Genomic Scale Height (cm)</t>
   </si>
   <si>
-    <t>Height in centimeters of the genomic scale field (full plot height will be influenced based on this value).Options: positive numeric value.</t>
-  </si>
-  <si>
     <t>annotation_height_cm</t>
   </si>
   <si>
@@ -283,9 +271,6 @@
     <t>Annotation Height (cm)</t>
   </si>
   <si>
-    <t>Height in centimeters of each line in the annotation track (full plot height will be influenced based on this value).Options: positive numeric value.</t>
-  </si>
-  <si>
     <t>spacer_height_cm</t>
   </si>
   <si>
@@ -295,18 +280,12 @@
     <t>Spacer Height (cm)</t>
   </si>
   <si>
-    <t>Height in centimeters of each spacer line used in the plot (full plot height will be influenced based on this value).Options: positive numeric value.</t>
-  </si>
-  <si>
     <t>track_width_cm</t>
   </si>
   <si>
     <t>tracks_width_in_cm</t>
   </si>
   <si>
-    <t>Specify the width in centimeters for the sequencing track window of the plot (full plot width will be determined based on this value).</t>
-  </si>
-  <si>
     <t>margin_width_cm</t>
   </si>
   <si>
@@ -316,9 +295,6 @@
     <t>margin_width_I</t>
   </si>
   <si>
-    <t>Specify the size in centimeters of the margins on each side of the sequencing tracks.</t>
-  </si>
-  <si>
     <t>panels_max_width_cm</t>
   </si>
   <si>
@@ -346,9 +322,6 @@
     <t>scale_per_space</t>
   </si>
   <si>
-    <t>Width in cm allocated to the tracks scale ('auto' or a positive numeric value). Ignored if 'Display track scales' is unticked.</t>
-  </si>
-  <si>
     <t>full_height_cm</t>
   </si>
   <si>
@@ -358,9 +331,6 @@
     <t>[*] Full Plot Height (cm)</t>
   </si>
   <si>
-    <t>Specify the plot height in centimeters. We recommend to set this argument to NULL to allow this to be determined automatically based on the number of tracks to display and the individual 'Tracks Heights'.</t>
-  </si>
-  <si>
     <t>full_width_cm</t>
   </si>
   <si>
@@ -466,18 +436,12 @@
     <t>panels_width_fixed</t>
   </si>
   <si>
-    <t>Specify if the tracks labels should mandatorily occupy all the space provided in the 'Plot display parameters' tab or if they can use less should it be possible. Ignored if 'Panels Width' is set to 'auto'</t>
-  </si>
-  <si>
     <t>horizontal_panels_list</t>
   </si>
   <si>
     <t>panel_horizontal</t>
   </si>
   <si>
-    <t>If left unticked, an automatic assignment based on available space will be performed. If ticked, tick which dataset and/or subgroup panels text should be displayed horizontally (if unticked they will be displayed vertically).</t>
-  </si>
-  <si>
     <t>print_one_line_sample_names</t>
   </si>
   <si>
@@ -544,9 +508,6 @@
     <t>[*] Detailed Panel Text Font Sizes</t>
   </si>
   <si>
-    <t>List of font sizes for each dataset and subgroup in the following format: dataset1:12,8,6,4;dataset2:12,6,4.</t>
-  </si>
-  <si>
     <t>incl_first_panel</t>
   </si>
   <si>
@@ -802,9 +763,6 @@
     <t>Display Feature Names</t>
   </si>
   <si>
-    <t>Display loci names in the annotation panel.</t>
-  </si>
-  <si>
     <t>center_of_mass</t>
   </si>
   <si>
@@ -826,9 +784,6 @@
     <t>Feature Names Above Features</t>
   </si>
   <si>
-    <t>If ticked, feature names are displayed above features. If unticked, feature names are displayed below features.</t>
-  </si>
-  <si>
     <t>feature_names_alternating</t>
   </si>
   <si>
@@ -955,9 +910,6 @@
     <t>For each dataset, specify whether to 'group' auto-scale or just auto-scale for each individual track.</t>
   </si>
   <si>
-    <t>Height in centimeters of each sequencing track (full plot height will be influenced by this value). Options: positive numeric value. Recommended value between 0.2 and 1.0 cm.</t>
-  </si>
-  <si>
     <t>R_help</t>
   </si>
   <si>
@@ -976,9 +928,6 @@
     <t>Prefix added before replicate numbers (e.g. rep, r). NULL will lead to display of individual replicates without separate naming. NA will lead to display of replicate numbers without a prefix. Ignored when the mean of replicates is calculated.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specify if horizontal,vertical line-separators should be displayed in order to clearly separate panels. Deselected and selected (FALSE,TRUE) by default for horizontal and vertical, respectively. If one logical value is supplied it will automatically be applied to both. Horizontal line-separators will only be displayed if 'Dataset Spacers' is selected. </t>
-  </si>
-  <si>
     <t>Integer value (&gt;1). Default: 'auto';  the bin size will be automatically determined. The lower the value, the slower the plotting.</t>
   </si>
   <si>
@@ -991,18 +940,9 @@
     <t>Header Font Color(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Font size of the genomic scale (integer value &gt;4). NULL will lead to automatic determination based on Genomic Scale Height (cm). </t>
-  </si>
-  <si>
-    <t>Font size(s) in the header region (integer value(s) &gt;4). One integer or three comma-separated integers for 'main title', 'genomic range (subtitle)' and 'scale', respectively. Will be determined automatically by default based on Title Field Height (cm).</t>
-  </si>
-  <si>
     <t>allow,all,none</t>
   </si>
   <si>
-    <t>Display reverse strand features as a miror of the forward strand, which is determined by selecting/deselecting the above tickbox 'Feature Names Above Features'. Will be ignored with 'Intermingled strands display'</t>
-  </si>
-  <si>
     <t>Number of bins to display per centimeter. Only relevant if 'Bin Size' is automatically determined.</t>
   </si>
   <si>
@@ -1366,9 +1306,6 @@
     <t>Height in centimeters of the title field (full plot height will be influenced by this value). Will be ignored if the field is set too small to fit the font size selected for the title.</t>
   </si>
   <si>
-    <t>Height in centimeters of the title field (full plot height will be influenced based on this value). Options: positive numeric value. Will be ignored if the field is set too small to fit the font size selected for the title.</t>
-  </si>
-  <si>
     <t>Pick colors for the individual sample tracks (replicates for a given sample will get the same color).</t>
   </si>
   <si>
@@ -1399,9 +1336,6 @@
     <t>Feature Name Font Size</t>
   </si>
   <si>
-    <t>If 'Tracks Width' is not specified, you can specify the width in centimeters for the full plot. We recommend to set this argument to NULL to allow this to be determined automatically based on the 'Tracks Width' and panel widths (determined under 'Panel display' tab).</t>
-  </si>
-  <si>
     <t>Panel display</t>
   </si>
   <si>
@@ -1415,6 +1349,81 @@
   </si>
   <si>
     <t>tracks_height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify a scaling factor to apply for on-screen display - ignored when exporting to pdf (pdf=TRUE). </t>
+  </si>
+  <si>
+    <t>Display reverse strand features as a miror of the forward strand. Will be ignored with 'Intermingled strands display'</t>
+  </si>
+  <si>
+    <t>If TRUE, feature names are displayed above features. If FALSE, feature names are displayed below features.</t>
+  </si>
+  <si>
+    <t>Display feature/locus names in the annotation panel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Font size of the genomic scale (integer value &gt;4). NULL will lead to automatic determination. </t>
+  </si>
+  <si>
+    <t>Font size(s) in the header region (integer value(s) &gt;4). One integer or three comma-separated integers for 'main title', 'genomic range (subtitle)' and 'scale', respectively. Will be determined automatically by default.</t>
+  </si>
+  <si>
+    <t>Exclude the 'Header Panel' at the top of the produced plot? This argument is ignored if a header is provided manually.</t>
+  </si>
+  <si>
+    <t>Specify a header to be used instead of the automatically generated header based on the name of the locus/feature. If genomic coordinates are used, the title panel will be excluded per default unless specified here.</t>
+  </si>
+  <si>
+    <t>Width in cm allocated to the tracks scale ('auto' or a positive numeric value). Ignored if incl_track_scales=FALSE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combine all sample 'subgroup' information in one panel - separated by points (.)  - instead of setting up multiple panels. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify if horizontal,vertical line-separators should be displayed in order to clearly separate panels. c(FALSE,TRUE) by default for horizontal and vertical, respectively. If one logical value is supplied it will automatically be applied to both. Horizontal line-separators will only be displayed if horizontal_spacers=TRUE. </t>
+  </si>
+  <si>
+    <t>List of font sizes for each dataset and subgroup in the following format: list('dataset1'=c(12,8,6,4), 'dataset2'=c(12,6,4), ...).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of boolean vectors indicating whether text in the individual subpanels in the 'sample overview panel' should be displayed horizontally (TRUE) or vertically (FALSE). The list should be provided in the following format: list('dataset1'=c(TRUE,FALSE,FALSE,TRUE), 'dataset2'=c(TRUE,TRUE), ...). If NULL, an automatic assignment based on available space will be performed. </t>
+  </si>
+  <si>
+    <t>Specify if the tracks labels should mandatorily occupy all the space provided in panels_max_width_cm or if they can use less should it be possible. Ignored if panels_max_width_cm='auto'.</t>
+  </si>
+  <si>
+    <t>Specify the size in centimeters of the margins on each side of the sequencing tracks. 0.05 cm per default.</t>
+  </si>
+  <si>
+    <t>Height in centimeters of each spacer line used in the plot (full plot height will be influenced based on this value).Positive numeric value. Default 0.06 cm.</t>
+  </si>
+  <si>
+    <t>Height in centimeters of each line in the annotation track (full plot height will be influenced based on this value). Positive numeric value. Default 0.24 cm.</t>
+  </si>
+  <si>
+    <t>Height in centimeters of the genomic scale field (full plot height will be influenced based on this value). Positive numeric value. Default 0.24 cm.</t>
+  </si>
+  <si>
+    <t>Height in centimeters of the title field (full plot height will be influenced based on this value). Positive numeric value. Default 0.66 cm. Will be ignored if the field is set too small to fit the font size selected for the title.</t>
+  </si>
+  <si>
+    <t>Height in centimeters of each sequencing track (full plot height will be influenced by this value). Positive numeric value. Default 0.3 cm. Recommended value between 0.2 and 1.0 cm.</t>
+  </si>
+  <si>
+    <t>If track_width_cm is not specified (=NULL), you can specify the width in centimeters for the full plot. We recommend to set this argument to NULL to allow this to be determined automatically based on the specified track_width_cm and panels_max_width_cm. Default NULL.</t>
+  </si>
+  <si>
+    <t>Specify the plot height in centimeters. We recommend to set this argument to NULL to allow this to be determined automatically based on the number of tracks to display and the specified track_height_cm. Default NULL.</t>
+  </si>
+  <si>
+    <t>Specify the width in centimeters for the sequencing track window of the plot (full plot width will be determined based on this value). Default 12 cm.</t>
+  </si>
+  <si>
+    <t>Number of bins to display per centimeter. Only relevant if 'Bin Size' is automatically determined. Default 250 bins/cm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra space up- and downstream of and relative to the selected genomic feature (0.1 = 10%). Only taken into account when locus/feature name is entered - ignored when genomic coordinates are entered.  Default c(1.5,1.5). </t>
   </si>
 </sst>
 </file>
@@ -1851,8 +1860,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1897,7 +1906,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1914,7 +1923,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>13</v>
@@ -1926,7 +1935,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>15</v>
@@ -1934,32 +1943,32 @@
     </row>
     <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>436</v>
+        <v>416</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="6" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>437</v>
+        <v>417</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1986,7 +1995,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="J4" s="15" t="s">
         <v>21</v>
@@ -2006,7 +2015,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>18</v>
@@ -2018,10 +2027,10 @@
         <v>26</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>27</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2029,7 +2038,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>17</v>
@@ -2042,16 +2051,16 @@
         <v>18</v>
       </c>
       <c r="G6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>31</v>
-      </c>
       <c r="J6" s="15" t="s">
-        <v>31</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2059,31 +2068,31 @@
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="I7" s="15" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>37</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2091,7 +2100,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>17</v>
@@ -2104,16 +2113,16 @@
         <v>18</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="J8" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2121,7 +2130,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>17</v>
@@ -2134,16 +2143,16 @@
         <v>18</v>
       </c>
       <c r="G9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="J9" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2151,31 +2160,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2183,28 +2192,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="J11" s="15"/>
     </row>
@@ -2213,7 +2222,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>17</v>
@@ -2226,16 +2235,16 @@
         <v>18</v>
       </c>
       <c r="G12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>50</v>
-      </c>
       <c r="J12" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2243,7 +2252,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>17</v>
@@ -2256,16 +2265,16 @@
         <v>18</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>54</v>
-      </c>
       <c r="J13" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2273,7 +2282,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>17</v>
@@ -2286,16 +2295,16 @@
         <v>18</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2303,7 +2312,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>17</v>
@@ -2316,16 +2325,16 @@
         <v>18</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>435</v>
+        <v>415</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -2333,29 +2342,29 @@
         <v>9</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2363,29 +2372,29 @@
         <v>9</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>65</v>
-      </c>
       <c r="J17" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2393,31 +2402,31 @@
         <v>9</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="H18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>69</v>
-      </c>
       <c r="I18" s="14" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>70</v>
+        <v>461</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2425,31 +2434,31 @@
         <v>9</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D19" s="9">
         <v>0.3</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>305</v>
+        <v>456</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2457,31 +2466,31 @@
         <v>9</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2489,127 +2498,127 @@
         <v>9</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>391</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="H22" s="8" t="s">
+      <c r="I23" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I22" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>393</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="C24" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D24" s="9">
         <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>445</v>
+        <v>424</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>88</v>
+        <v>459</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2617,31 +2626,31 @@
         <v>9</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>92</v>
+        <v>451</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2649,31 +2658,31 @@
         <v>9</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2681,7 +2690,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>17</v>
@@ -2691,19 +2700,19 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2711,31 +2720,31 @@
         <v>9</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>102</v>
+        <v>445</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2743,31 +2752,31 @@
         <v>9</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>106</v>
+        <v>458</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -2775,39 +2784,39 @@
         <v>9</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>17</v>
@@ -2817,27 +2826,27 @@
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>17</v>
@@ -2847,59 +2856,59 @@
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F33" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G33" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>122</v>
-      </c>
       <c r="I33" s="15" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>17</v>
@@ -2909,27 +2918,27 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>17</v>
@@ -2939,27 +2948,27 @@
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>23</v>
@@ -2968,30 +2977,30 @@
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>17</v>
@@ -3001,27 +3010,27 @@
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>17</v>
@@ -3031,19 +3040,19 @@
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -3051,7 +3060,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>17</v>
@@ -3061,49 +3070,49 @@
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="J40" s="14" t="s">
-        <v>145</v>
+        <v>449</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3111,7 +3120,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>17</v>
@@ -3121,19 +3130,19 @@
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="J41" s="14" t="s">
-        <v>149</v>
+        <v>446</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3141,7 +3150,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>17</v>
@@ -3151,19 +3160,19 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3171,29 +3180,29 @@
         <v>9</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C43" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3201,31 +3210,31 @@
         <v>9</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -3233,31 +3242,31 @@
         <v>9</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="J45" s="14" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3265,31 +3274,31 @@
         <v>9</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>168</v>
+        <v>448</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3297,7 +3306,7 @@
         <v>9</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>17</v>
@@ -3307,19 +3316,19 @@
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3327,7 +3336,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>17</v>
@@ -3337,19 +3346,19 @@
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="J48" s="14" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -3357,31 +3366,31 @@
         <v>9</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>312</v>
+        <v>447</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3389,31 +3398,31 @@
         <v>9</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3421,31 +3430,31 @@
         <v>9</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="J51" s="14" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3453,7 +3462,7 @@
         <v>9</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>17</v>
@@ -3463,19 +3472,19 @@
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="J52" s="14" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3483,31 +3492,31 @@
         <v>9</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="J53" s="14" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3515,31 +3524,31 @@
         <v>9</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3547,31 +3556,31 @@
         <v>9</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>455</v>
+        <v>433</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="J55" s="15" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -3579,31 +3588,31 @@
         <v>9</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>455</v>
+        <v>433</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="J56" s="15" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3611,7 +3620,7 @@
         <v>9</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>23</v>
@@ -3620,22 +3629,22 @@
         <v>250</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>455</v>
+        <v>433</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="J57" s="15" t="s">
-        <v>321</v>
+        <v>460</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3643,31 +3652,31 @@
         <v>9</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="J58" s="14" t="s">
-        <v>318</v>
+        <v>442</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3675,31 +3684,31 @@
         <v>9</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="J59" s="14" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3707,29 +3716,29 @@
         <v>9</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="6" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="I60" s="14" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="J60" s="14" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3737,39 +3746,39 @@
         <v>9</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="I61" s="14" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="J61" s="14" t="s">
-        <v>317</v>
+        <v>441</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>17</v>
@@ -3779,51 +3788,51 @@
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="7" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>415</v>
+        <v>395</v>
       </c>
       <c r="J62" s="15" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>416</v>
+        <v>396</v>
       </c>
       <c r="J63" s="15" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3831,31 +3840,31 @@
         <v>9</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>417</v>
+        <v>397</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3863,29 +3872,29 @@
         <v>9</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="7" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="I65" s="15" t="s">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="J65" s="15" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3893,71 +3902,71 @@
         <v>9</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="I66" s="15" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="J66" s="15" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
       <c r="J67" s="14" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>17</v>
@@ -3967,19 +3976,19 @@
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="J68" s="14" t="s">
-        <v>254</v>
+        <v>440</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -3987,7 +3996,7 @@
         <v>9</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>17</v>
@@ -3997,27 +4006,27 @@
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="J69" s="14" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>17</v>
@@ -4027,19 +4036,19 @@
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H70" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="G70" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="H70" s="8" t="s">
-        <v>261</v>
-      </c>
       <c r="I70" s="14" t="s">
-        <v>428</v>
+        <v>408</v>
       </c>
       <c r="J70" s="14" t="s">
-        <v>262</v>
+        <v>439</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -4047,7 +4056,7 @@
         <v>9</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>17</v>
@@ -4057,27 +4066,27 @@
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="I71" s="14" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="J71" s="14" t="s">
-        <v>320</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>17</v>
@@ -4087,49 +4096,49 @@
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="H72" s="8" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="J72" s="14" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>430</v>
+        <v>410</v>
       </c>
       <c r="J73" s="14" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4137,29 +4146,29 @@
         <v>9</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>451</v>
+        <v>430</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="J74" s="14" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4167,31 +4176,31 @@
         <v>9</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="J75" s="14" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4199,29 +4208,29 @@
         <v>9</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
       <c r="J76" s="14" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4229,39 +4238,39 @@
         <v>9</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="I77" s="14" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="J77" s="14" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>17</v>
@@ -4271,19 +4280,19 @@
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>422</v>
+        <v>402</v>
       </c>
       <c r="J78" s="14" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -4291,31 +4300,31 @@
         <v>9</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="H79" s="8" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="I79" s="14" t="s">
-        <v>419</v>
+        <v>399</v>
       </c>
       <c r="J79" s="14" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4323,31 +4332,31 @@
         <v>9</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="I80" s="14" t="s">
-        <v>418</v>
+        <v>398</v>
       </c>
       <c r="J80" s="14" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>